<commit_message>
add longitude latitude for locations and start sorting on python
</commit_message>
<xml_diff>
--- a/Locations.xlsx
+++ b/Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Lee\Documents\GitHub\JSA-Ride-Groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06C7B5-98A6-4BBE-A9B8-563A86651C2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46B24B6-A539-4A33-B276-C146E0C41A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69F491A2-B1CE-4F4D-B688-3010BBE37461}"/>
+    <workbookView xWindow="3696" yWindow="1044" windowWidth="17280" windowHeight="8964" xr2:uid="{69F491A2-B1CE-4F4D-B688-3010BBE37461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,131 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>Revelle</t>
+  </si>
+  <si>
+    <t>ERC</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Muir</t>
+  </si>
+  <si>
+    <t>La Jolla Village Tennis Club</t>
+  </si>
+  <si>
+    <t>Axiom</t>
+  </si>
+  <si>
+    <t>Whole Foods</t>
+  </si>
+  <si>
+    <t>La Jolla Palms</t>
+  </si>
+  <si>
+    <t>Costa Verde</t>
+  </si>
+  <si>
+    <t>Pines of La Jolla</t>
+  </si>
+  <si>
+    <t>Vons</t>
+  </si>
+  <si>
+    <t>International Gardens</t>
+  </si>
+  <si>
+    <t>La Jolla Crossroads</t>
+  </si>
+  <si>
+    <t>La Regencia</t>
+  </si>
+  <si>
+    <t>Ralphs</t>
+  </si>
+  <si>
+    <t>Playmor Terrace</t>
+  </si>
+  <si>
+    <t>Verano</t>
+  </si>
+  <si>
+    <t>Via Marin</t>
+  </si>
+  <si>
+    <t>Camino Aguilla</t>
+  </si>
+  <si>
+    <t>Solazzo</t>
+  </si>
+  <si>
+    <t>Easter Way</t>
+  </si>
+  <si>
+    <t>UTC</t>
+  </si>
+  <si>
+    <t>Villas of Renaissance</t>
+  </si>
+  <si>
+    <t>Gilman Bus Stop</t>
+  </si>
+  <si>
+    <t>Mesa Nueva</t>
+  </si>
+  <si>
+    <t>Regents Courts</t>
+  </si>
+  <si>
+    <t>Pacific Regent</t>
+  </si>
+  <si>
+    <t>La Scala</t>
+  </si>
+  <si>
+    <t>Del Sol</t>
+  </si>
+  <si>
+    <t>Nobel Court</t>
+  </si>
+  <si>
+    <t>Villa La Jolla</t>
+  </si>
+  <si>
+    <t>Venetian</t>
+  </si>
+  <si>
+    <t>Valentia</t>
+  </si>
+  <si>
+    <t>International House</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,8 +186,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +505,688 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F62829-06EC-4194-8773-0BB7E53DE3F1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>32.869822999999997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-117.221839</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1">
+        <v>32.861474000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-117.220888</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>32.870277999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-117.216748</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32.865586999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-117.223051</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1">
+        <v>32.880310000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-117.211805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>32.886178000000001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-117.242307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1">
+        <v>32.877268000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-117.235472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32.866813</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-117.223741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1">
+        <v>32.88411</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-117.242165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>32.872374999999998</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-117.203283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>32.870009000000003</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-117.223598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>32.871130999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-117.222324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1">
+        <v>32.864677999999998</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-117.224298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1">
+        <v>32.868065000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-117.223664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1">
+        <v>32.881476999999997</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-117.241263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1">
+        <v>32.875391</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-117.223173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1">
+        <v>32.878554999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-117.240646</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1">
+        <v>32.867497</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-117.227152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1">
+        <v>32.869123000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-117.223113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <v>32.866790999999999</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-117.22093099999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>32.862718999999998</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-117.217811</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <v>32.866565999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-117.23176100000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1">
+        <v>32.867341000000003</v>
+      </c>
+      <c r="C24" s="1">
+        <v>-117.219014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>32.875368999999999</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-117.24185199999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>32.878070999999998</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-117.233491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>32.864679000000002</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-117.23572299999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>32.869615000000003</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-117.213624</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1">
+        <v>32.868532000000002</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-117.20229399999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1">
+        <v>32.867834000000002</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-117.221236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="1">
+        <v>32.865139999999997</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-117.22711099999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="1">
+        <v>32.856233000000003</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-117.233334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1">
+        <v>32.862960000000001</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-117.233986</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1">
+        <v>32.888191999999997</v>
+      </c>
+      <c r="C34" s="1">
+        <v>-117.242526</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="1">
+        <v>32.870553000000001</v>
+      </c>
+      <c r="C35" s="1">
+        <v>-117.202547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>32.862644000000003</v>
+      </c>
+      <c r="C36" s="1">
+        <v>-117.223522</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1">
+        <v>32.882497999999998</v>
+      </c>
+      <c r="C37" s="1">
+        <v>-117.233301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1">
+        <v>32.868768000000003</v>
+      </c>
+      <c r="C38" s="1">
+        <v>-117.230751</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A38">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>